<commit_message>
fix: precedence parsing accepts function calls
</commit_message>
<xml_diff>
--- a/doc/lltable.xlsx
+++ b/doc/lltable.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="93">
   <si>
     <t xml:space="preserve">if </t>
   </si>
@@ -241,19 +241,22 @@
     <t xml:space="preserve">expression</t>
   </si>
   <si>
-    <t xml:space="preserve">(4, 5)</t>
+    <t xml:space="preserve">(4, 19)</t>
   </si>
   <si>
     <t xml:space="preserve">args</t>
   </si>
   <si>
-    <t xml:space="preserve">(4, 7)</t>
+    <t xml:space="preserve">(4, 21)</t>
   </si>
   <si>
     <t xml:space="preserve">args2</t>
   </si>
   <si>
-    <t xml:space="preserve">(4, 9)</t>
+    <t xml:space="preserve">(4, 24)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(4, 23)</t>
   </si>
   <si>
     <t xml:space="preserve">codeBlock</t>
@@ -776,8 +779,8 @@
   </sheetPr>
   <dimension ref="A1:AM17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AG1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:AM17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N13" activeCellId="0" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2239,7 +2242,7 @@
         <v>40</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="K13" s="8" t="s">
         <v>40</v>
@@ -2251,7 +2254,7 @@
         <v>40</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O13" s="8" t="s">
         <v>40</v>
@@ -2331,22 +2334,22 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>40</v>
@@ -2355,7 +2358,7 @@
         <v>40</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>40</v>
@@ -2364,10 +2367,10 @@
         <v>40</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M14" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N14" s="8" t="s">
         <v>40</v>
@@ -2379,7 +2382,7 @@
         <v>40</v>
       </c>
       <c r="Q14" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="R14" s="10" t="s">
         <v>42</v>
@@ -2418,28 +2421,28 @@
         <v>40</v>
       </c>
       <c r="AD14" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AE14" s="8" t="s">
         <v>40</v>
       </c>
       <c r="AF14" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AG14" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AH14" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AI14" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AJ14" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AK14" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AL14" s="8" t="s">
         <v>40</v>
@@ -2450,22 +2453,22 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>40</v>
@@ -2474,7 +2477,7 @@
         <v>40</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>40</v>
@@ -2483,10 +2486,10 @@
         <v>40</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="M15" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="N15" s="8" t="s">
         <v>40</v>
@@ -2498,7 +2501,7 @@
         <v>40</v>
       </c>
       <c r="Q15" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="R15" s="10" t="s">
         <v>42</v>
@@ -2537,31 +2540,31 @@
         <v>40</v>
       </c>
       <c r="AD15" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AE15" s="8" t="s">
         <v>40</v>
       </c>
       <c r="AF15" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AG15" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AH15" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AI15" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AJ15" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AK15" s="10" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AL15" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AM15" s="8" t="s">
         <v>40</v>
@@ -2569,7 +2572,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>40</v>
@@ -2665,19 +2668,19 @@
         <v>40</v>
       </c>
       <c r="AG16" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AH16" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AI16" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AJ16" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AK16" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AL16" s="8" t="s">
         <v>40</v>
@@ -2688,7 +2691,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>40</v>
@@ -2784,16 +2787,16 @@
         <v>40</v>
       </c>
       <c r="AG17" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AH17" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AI17" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AJ17" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AK17" s="8" t="s">
         <v>40</v>

</xml_diff>